<commit_message>
recent updates to trendscanning code
</commit_message>
<xml_diff>
--- a/factor_returns_momentum.xlsx
+++ b/factor_returns_momentum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://resbank-my.sharepoint.com/personal/cathy_hlungwani_resbank_co_za/Documents/Documents/1. MEng - Data Science/1. Project_2025/Data/factor_timing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{DB9EABAB-D155-4145-86E8-321E1299B916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6913A415-EFE9-4108-AB4B-FCA3885A0C74}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{286247A6-C373-4255-86C0-EB0E92DADCE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{212E4862-DA6A-4B5A-B4E4-F3B2B06FB1F3}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{86B4F7FB-E57C-4017-86C8-FFB9EF78BA53}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{CE833FA7-6B75-497D-9FC5-06770AF9F191}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -38,10 +38,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Momentum</t>
+    <t>Date</t>
   </si>
   <si>
-    <t>Date</t>
+    <t>Return</t>
   </si>
 </sst>
 </file>
@@ -427,11 +427,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049526AD-85CE-4F0F-84DD-1488887E03E6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129A4DFA-7223-4318-844A-DD8F2DA2B975}">
   <dimension ref="A1:B243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -441,1946 +441,1943 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>37987</v>
+        <v>38018</v>
       </c>
       <c r="B2" s="2">
-        <v>1.03E-2</v>
+        <v>2.2127789077706961E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>38018</v>
+        <v>38047</v>
       </c>
       <c r="B3" s="2">
-        <v>1.5699999999999999E-2</v>
+        <v>-1.6655635729127649E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>38047</v>
+        <v>38078</v>
       </c>
       <c r="B4" s="2">
-        <v>1.47E-2</v>
+        <v>2.5778560297974429E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>38078</v>
+        <v>38108</v>
       </c>
       <c r="B5" s="2">
-        <v>-2.2700000000000001E-2</v>
+        <v>-1.9048492809268902E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>38108</v>
+        <v>38139</v>
       </c>
       <c r="B6" s="2">
-        <v>1.8E-3</v>
+        <v>1.5293234403315203E-3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>38139</v>
+        <v>38169</v>
       </c>
       <c r="B7" s="2">
-        <v>3.5000000000000001E-3</v>
+        <v>-2.6884256516272131E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>38169</v>
+        <v>38200</v>
       </c>
       <c r="B8" s="2">
-        <v>1.2200000000000001E-2</v>
+        <v>-5.5705554594220219E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>38200</v>
+        <v>38231</v>
       </c>
       <c r="B9" s="2">
-        <v>7.0599999999999996E-2</v>
+        <v>1.447962643273959E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>38231</v>
+        <v>38261</v>
       </c>
       <c r="B10" s="2">
-        <v>6.54E-2</v>
+        <v>1.7173912837536331E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>38261</v>
+        <v>38292</v>
       </c>
       <c r="B11" s="2">
-        <v>4.58E-2</v>
+        <v>-9.7732153347419359E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>38292</v>
+        <v>38322</v>
       </c>
       <c r="B12" s="2">
-        <v>0.1181</v>
+        <v>4.4200347184313316E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>38322</v>
+        <v>38353</v>
       </c>
       <c r="B13" s="2">
-        <v>4.1099999999999998E-2</v>
+        <v>2.3562176707877747E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>38353</v>
+        <v>38384</v>
       </c>
       <c r="B14" s="2">
-        <v>2.0999999999999999E-3</v>
+        <v>-3.4444601371806716E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>38384</v>
+        <v>38412</v>
       </c>
       <c r="B15" s="2">
-        <v>4.2000000000000003E-2</v>
+        <v>8.065587390690665E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>38412</v>
+        <v>38443</v>
       </c>
       <c r="B16" s="2">
-        <v>-3.5299999999999998E-2</v>
+        <v>7.5204334451813848E-3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>38443</v>
+        <v>38473</v>
       </c>
       <c r="B17" s="2">
-        <v>-2.58E-2</v>
+        <v>-0.12195622529831718</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>38473</v>
+        <v>38504</v>
       </c>
       <c r="B18" s="2">
-        <v>8.6800000000000002E-2</v>
+        <v>6.145977126378388E-2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>38504</v>
+        <v>38534</v>
       </c>
       <c r="B19" s="2">
-        <v>1.77E-2</v>
+        <v>-5.0321319968054556E-2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>38534</v>
+        <v>38565</v>
       </c>
       <c r="B20" s="2">
-        <v>8.2199999999999995E-2</v>
+        <v>4.8111864606293464E-2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
-        <v>38565</v>
+        <v>38596</v>
       </c>
       <c r="B21" s="2">
-        <v>3.0599999999999999E-2</v>
+        <v>-7.1606270256113547E-2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
-        <v>38596</v>
+        <v>38626</v>
       </c>
       <c r="B22" s="2">
-        <v>9.2999999999999999E-2</v>
+        <v>0.1256152201667744</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>38626</v>
+        <v>38657</v>
       </c>
       <c r="B23" s="2">
-        <v>-3.6400000000000002E-2</v>
+        <v>-6.0733594899460508E-2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>38657</v>
+        <v>38687</v>
       </c>
       <c r="B24" s="2">
-        <v>3.2199999999999999E-2</v>
+        <v>-5.193586494482072E-2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>38687</v>
+        <v>38718</v>
       </c>
       <c r="B25" s="2">
-        <v>0.08</v>
+        <v>-2.2701336174935305E-2</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
-        <v>38718</v>
+        <v>38749</v>
       </c>
       <c r="B26" s="2">
-        <v>0.1108</v>
+        <v>0.1169731834562</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
-        <v>38749</v>
+        <v>38777</v>
       </c>
       <c r="B27" s="2">
-        <v>-2.63E-2</v>
+        <v>-0.10404491068509925</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
-        <v>38777</v>
+        <v>38808</v>
       </c>
       <c r="B28" s="2">
-        <v>8.09E-2</v>
+        <v>5.1689760652661398E-2</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
-        <v>38808</v>
+        <v>38838</v>
       </c>
       <c r="B29" s="2">
-        <v>1.77E-2</v>
+        <v>6.7543688332059149E-2</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
-        <v>38838</v>
+        <v>38869</v>
       </c>
       <c r="B30" s="2">
-        <v>-4.1099999999999998E-2</v>
+        <v>-8.748645426936319E-2</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
-        <v>38869</v>
+        <v>38899</v>
       </c>
       <c r="B31" s="2">
-        <v>4.2900000000000001E-2</v>
+        <v>3.7157509602840255E-2</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
-        <v>38899</v>
+        <v>38930</v>
       </c>
       <c r="B32" s="2">
-        <v>-2.1899999999999999E-2</v>
+        <v>-5.9465387163058714E-2</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
-        <v>38930</v>
+        <v>38961</v>
       </c>
       <c r="B33" s="2">
-        <v>5.0900000000000001E-2</v>
+        <v>2.4512343127714997E-2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
-        <v>38961</v>
+        <v>38991</v>
       </c>
       <c r="B34" s="2">
-        <v>2.6700000000000002E-2</v>
+        <v>-2.7094934534488635E-2</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
-        <v>38991</v>
+        <v>39022</v>
       </c>
       <c r="B35" s="2">
-        <v>4.8000000000000001E-2</v>
+        <v>2.2007063094861889E-2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
-        <v>39022</v>
+        <v>39052</v>
       </c>
       <c r="B36" s="2">
-        <v>3.2000000000000001E-2</v>
+        <v>-3.4010459735251741E-2</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
-        <v>39052</v>
+        <v>39083</v>
       </c>
       <c r="B37" s="2">
-        <v>7.0999999999999994E-2</v>
+        <v>1.7955237883465536E-2</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
-        <v>39083</v>
+        <v>39114</v>
       </c>
       <c r="B38" s="2">
-        <v>3.7699999999999997E-2</v>
+        <v>1.4607021045963009E-2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
-        <v>39114</v>
+        <v>39142</v>
       </c>
       <c r="B39" s="2">
-        <v>1.7000000000000001E-2</v>
+        <v>-5.9097662876170132E-2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
-        <v>39142</v>
+        <v>39173</v>
       </c>
       <c r="B40" s="2">
-        <v>7.2499999999999995E-2</v>
+        <v>1.1269673580662332E-2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
-        <v>39173</v>
+        <v>39203</v>
       </c>
       <c r="B41" s="2">
-        <v>4.7699999999999999E-2</v>
+        <v>5.2401518307059858E-2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
-        <v>39203</v>
+        <v>39234</v>
       </c>
       <c r="B42" s="2">
-        <v>-5.7999999999999996E-3</v>
+        <v>1.6124743043649636E-2</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
-        <v>39234</v>
+        <v>39264</v>
       </c>
       <c r="B43" s="2">
-        <v>-1.7999999999999999E-2</v>
+        <v>-2.4972582278942168E-2</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
-        <v>39264</v>
+        <v>39295</v>
       </c>
       <c r="B44" s="2">
-        <v>7.3000000000000001E-3</v>
+        <v>-6.6533281893812468E-3</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
-        <v>39295</v>
+        <v>39326</v>
       </c>
       <c r="B45" s="2">
-        <v>1.1299999999999999E-2</v>
+        <v>-1.9893867874305471E-2</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
-        <v>39326</v>
+        <v>39356</v>
       </c>
       <c r="B46" s="2">
-        <v>2.8000000000000001E-2</v>
+        <v>-4.8862627884215915E-2</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
-        <v>39356</v>
+        <v>39387</v>
       </c>
       <c r="B47" s="2">
-        <v>7.9000000000000001E-2</v>
+        <v>9.3783268171851342E-2</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
-        <v>39387</v>
+        <v>39417</v>
       </c>
       <c r="B48" s="2">
-        <v>-2.5700000000000001E-2</v>
+        <v>-2.8387907643475652E-3</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
-        <v>39417</v>
+        <v>39448</v>
       </c>
       <c r="B49" s="2">
-        <v>-3.0300000000000001E-2</v>
+        <v>2.3657840058880608E-2</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
-        <v>39448</v>
+        <v>39479</v>
       </c>
       <c r="B50" s="2">
-        <v>-5.91E-2</v>
+        <v>-0.20147166638761327</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
-        <v>39479</v>
+        <v>39508</v>
       </c>
       <c r="B51" s="2">
-        <v>0.13139999999999999</v>
+        <v>0.14306605292829355</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
-        <v>39508</v>
+        <v>39539</v>
       </c>
       <c r="B52" s="2">
-        <v>-3.3700000000000001E-2</v>
+        <v>-8.9053388177761983E-2</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
-        <v>39539</v>
+        <v>39569</v>
       </c>
       <c r="B53" s="2">
-        <v>5.5E-2</v>
+        <v>-1.2160442030342944E-2</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
-        <v>39569</v>
+        <v>39600</v>
       </c>
       <c r="B54" s="2">
-        <v>5.1400000000000001E-2</v>
+        <v>7.5775950574877071E-2</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
-        <v>39600</v>
+        <v>39630</v>
       </c>
       <c r="B55" s="2">
-        <v>-4.7699999999999999E-2</v>
+        <v>6.2119721004096684E-2</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
-        <v>39630</v>
+        <v>39661</v>
       </c>
       <c r="B56" s="2">
-        <v>-0.12770000000000001</v>
+        <v>-7.7587925331008445E-2</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
-        <v>39661</v>
+        <v>39692</v>
       </c>
       <c r="B57" s="2">
-        <v>2.7099999999999999E-2</v>
+        <v>0.12246997241056679</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
-        <v>39692</v>
+        <v>39722</v>
       </c>
       <c r="B58" s="2">
-        <v>-0.1099</v>
+        <v>-3.3338741016329498E-2</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
-        <v>39722</v>
+        <v>39753</v>
       </c>
       <c r="B59" s="2">
-        <v>-7.1599999999999997E-2</v>
+        <v>-0.10328803631169847</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
-        <v>39753</v>
+        <v>39783</v>
       </c>
       <c r="B60" s="2">
-        <v>-1.5900000000000001E-2</v>
+        <v>-3.823163108382821E-2</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
-        <v>39783</v>
+        <v>39814</v>
       </c>
       <c r="B61" s="2">
-        <v>4.6899999999999997E-2</v>
+        <v>3.0990773538879135E-2</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
-        <v>39814</v>
+        <v>39845</v>
       </c>
       <c r="B62" s="2">
-        <v>-1.1999999999999999E-3</v>
+        <v>2.2666832006700055E-2</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
-        <v>39845</v>
+        <v>39873</v>
       </c>
       <c r="B63" s="2">
-        <v>-6.9900000000000004E-2</v>
+        <v>-0.17255321772391674</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
-        <v>39873</v>
+        <v>39904</v>
       </c>
       <c r="B64" s="2">
-        <v>7.7899999999999997E-2</v>
+        <v>0.12004207883586471</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
-        <v>39904</v>
+        <v>39934</v>
       </c>
       <c r="B65" s="2">
-        <v>-1.4E-2</v>
+        <v>-6.1591045324322247E-2</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
-        <v>39934</v>
+        <v>39965</v>
       </c>
       <c r="B66" s="2">
-        <v>8.5300000000000001E-2</v>
+        <v>0.10578035269002395</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
-        <v>39965</v>
+        <v>39995</v>
       </c>
       <c r="B67" s="2">
-        <v>-1.9400000000000001E-2</v>
+        <v>-0.1050607230081525</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
-        <v>39995</v>
+        <v>40026</v>
       </c>
       <c r="B68" s="2">
-        <v>9.1700000000000004E-2</v>
+        <v>4.1791044201576533E-2</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
-        <v>40026</v>
+        <v>40057</v>
       </c>
       <c r="B69" s="2">
-        <v>4.8099999999999997E-2</v>
+        <v>4.1206082472485361E-2</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
-        <v>40057</v>
+        <v>40087</v>
       </c>
       <c r="B70" s="2">
-        <v>-2.9999999999999997E-4</v>
+        <v>-4.6396406658237854E-2</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
-        <v>40087</v>
+        <v>40118</v>
       </c>
       <c r="B71" s="2">
-        <v>5.0299999999999997E-2</v>
+        <v>4.4400815303247798E-2</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
-        <v>40118</v>
+        <v>40148</v>
       </c>
       <c r="B72" s="2">
-        <v>0</v>
+        <v>-4.8448130497244168E-2</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
-        <v>40148</v>
+        <v>40179</v>
       </c>
       <c r="B73" s="2">
-        <v>5.2999999999999999E-2</v>
+        <v>6.6175102390703899E-2</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
-        <v>40179</v>
+        <v>40210</v>
       </c>
       <c r="B74" s="2">
-        <v>-2.76E-2</v>
+        <v>-3.9193841439730592E-2</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
-        <v>40210</v>
+        <v>40238</v>
       </c>
       <c r="B75" s="2">
-        <v>1.2999999999999999E-2</v>
+        <v>-7.2246679592826046E-2</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
-        <v>40238</v>
+        <v>40269</v>
       </c>
       <c r="B76" s="2">
-        <v>8.2299999999999998E-2</v>
+        <v>6.8553129880476016E-2</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
-        <v>40269</v>
+        <v>40299</v>
       </c>
       <c r="B77" s="2">
-        <v>5.9999999999999995E-4</v>
+        <v>5.1087804443258888E-2</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
-        <v>40299</v>
+        <v>40330</v>
       </c>
       <c r="B78" s="2">
-        <v>-4.53E-2</v>
+        <v>-1.2455414558511513E-2</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
-        <v>40330</v>
+        <v>40360</v>
       </c>
       <c r="B79" s="2">
-        <v>-3.1899999999999998E-2</v>
+        <v>-0.11079517525718185</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
-        <v>40360</v>
+        <v>40391</v>
       </c>
       <c r="B80" s="2">
-        <v>7.8E-2</v>
+        <v>0.11666983574082168</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
-        <v>40391</v>
+        <v>40422</v>
       </c>
       <c r="B81" s="2">
-        <v>-3.2899999999999999E-2</v>
+        <v>-0.13576108399152242</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
-        <v>40422</v>
+        <v>40452</v>
       </c>
       <c r="B82" s="2">
-        <v>0.1056</v>
+        <v>7.2830995380092522E-2</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
-        <v>40452</v>
+        <v>40483</v>
       </c>
       <c r="B83" s="2">
-        <v>1.49E-2</v>
+        <v>3.0241080452336422E-2</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
-        <v>40483</v>
+        <v>40513</v>
       </c>
       <c r="B84" s="2">
-        <v>-6.7000000000000002E-3</v>
+        <v>-7.0445503929154829E-2</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
-        <v>40513</v>
+        <v>40544</v>
       </c>
       <c r="B85" s="2">
-        <v>6.3100000000000003E-2</v>
+        <v>0.10804256243445975</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
-        <v>40544</v>
+        <v>40575</v>
       </c>
       <c r="B86" s="2">
-        <v>-4.3799999999999999E-2</v>
+        <v>-6.0357662547509405E-2</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
-        <v>40575</v>
+        <v>40603</v>
       </c>
       <c r="B87" s="2">
-        <v>2.75E-2</v>
+        <v>3.1647749549148507E-3</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
-        <v>40603</v>
+        <v>40634</v>
       </c>
       <c r="B88" s="2">
-        <v>1.6899999999999998E-2</v>
+        <v>-1.1735368964226334E-2</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
-        <v>40634</v>
+        <v>40664</v>
       </c>
       <c r="B89" s="2">
-        <v>2.9399999999999999E-2</v>
+        <v>3.6627531399355484E-2</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
-        <v>40664</v>
+        <v>40695</v>
       </c>
       <c r="B90" s="2">
-        <v>-1.0699999999999999E-2</v>
+        <v>-3.2531801344922728E-3</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
-        <v>40695</v>
+        <v>40725</v>
       </c>
       <c r="B91" s="2">
-        <v>-4.7000000000000002E-3</v>
+        <v>-9.9934521222341255E-3</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
-        <v>40725</v>
+        <v>40756</v>
       </c>
       <c r="B92" s="2">
-        <v>-5.3E-3</v>
+        <v>-2.7251180706100775E-2</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
-        <v>40756</v>
+        <v>40787</v>
       </c>
       <c r="B93" s="2">
-        <v>1.2500000000000001E-2</v>
+        <v>3.5648051334827513E-2</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
-        <v>40787</v>
+        <v>40817</v>
       </c>
       <c r="B94" s="2">
-        <v>-3.0800000000000001E-2</v>
+        <v>-0.11035834018753565</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
-        <v>40817</v>
+        <v>40848</v>
       </c>
       <c r="B95" s="2">
-        <v>7.7200000000000005E-2</v>
+        <v>4.7504567215942872E-2</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
-        <v>40848</v>
+        <v>40878</v>
       </c>
       <c r="B96" s="2">
-        <v>2.9100000000000001E-2</v>
+        <v>2.40532706817016E-2</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
-        <v>40878</v>
+        <v>40909</v>
       </c>
       <c r="B97" s="2">
-        <v>-4.4999999999999997E-3</v>
+        <v>-4.5852993625879579E-2</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
-        <v>40909</v>
+        <v>40940</v>
       </c>
       <c r="B98" s="2">
-        <v>3.2099999999999997E-2</v>
+        <v>1.1276719393090051E-2</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
-        <v>40940</v>
+        <v>40969</v>
       </c>
       <c r="B99" s="2">
-        <v>3.4000000000000002E-2</v>
+        <v>8.3633967108636131E-3</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
-        <v>40969</v>
+        <v>41000</v>
       </c>
       <c r="B100" s="2">
-        <v>1.9699999999999999E-2</v>
+        <v>-3.9068120093628034E-2</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
-        <v>41000</v>
+        <v>41030</v>
       </c>
       <c r="B101" s="2">
-        <v>3.9300000000000002E-2</v>
+        <v>5.3109508278313733E-2</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
-        <v>41030</v>
+        <v>41061</v>
       </c>
       <c r="B102" s="2">
-        <v>-2.5899999999999999E-2</v>
+        <v>-5.9215734972975387E-2</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
-        <v>41061</v>
+        <v>41091</v>
       </c>
       <c r="B103" s="2">
-        <v>2.81E-2</v>
+        <v>-4.4336331213972402E-2</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
-        <v>41091</v>
+        <v>41122</v>
       </c>
       <c r="B104" s="2">
-        <v>6.6500000000000004E-2</v>
+        <v>3.125335840610699E-3</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
-        <v>41122</v>
+        <v>41153</v>
       </c>
       <c r="B105" s="2">
-        <v>2.8799999999999999E-2</v>
+        <v>2.8291449523782597E-2</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
-        <v>41153</v>
+        <v>41183</v>
       </c>
       <c r="B106" s="2">
-        <v>-1.1999999999999999E-3</v>
+        <v>-2.2324129195346432E-2</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
-        <v>41183</v>
+        <v>41214</v>
       </c>
       <c r="B107" s="2">
-        <v>3.4299999999999997E-2</v>
+        <v>1.5459949950129115E-2</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
-        <v>41214</v>
+        <v>41244</v>
       </c>
       <c r="B108" s="2">
-        <v>1.7399999999999999E-2</v>
+        <v>-1.562069513195441E-2</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
-        <v>41244</v>
+        <v>41275</v>
       </c>
       <c r="B109" s="2">
-        <v>3.6999999999999998E-2</v>
+        <v>4.5723126302849471E-2</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
-        <v>41275</v>
+        <v>41306</v>
       </c>
       <c r="B110" s="2">
-        <v>-2.3999999999999998E-3</v>
+        <v>3.1964692789200222E-2</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
-        <v>41306</v>
+        <v>41334</v>
       </c>
       <c r="B111" s="2">
-        <v>-1.6899999999999998E-2</v>
+        <v>-4.0199652746939929E-2</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
-        <v>41334</v>
+        <v>41365</v>
       </c>
       <c r="B112" s="2">
-        <v>2.9100000000000001E-2</v>
+        <v>1.2005078415706194E-2</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
-        <v>41365</v>
+        <v>41395</v>
       </c>
       <c r="B113" s="2">
-        <v>2.0000000000000001E-4</v>
+        <v>-8.1074731246118303E-2</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
-        <v>41395</v>
+        <v>41426</v>
       </c>
       <c r="B114" s="2">
-        <v>6.4299999999999996E-2</v>
+        <v>0.11380683740578368</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
-        <v>41426</v>
+        <v>41456</v>
       </c>
       <c r="B115" s="2">
-        <v>-4.6800000000000001E-2</v>
+        <v>-6.4643587013935799E-2</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
-        <v>41456</v>
+        <v>41487</v>
       </c>
       <c r="B116" s="2">
-        <v>2.47E-2</v>
+        <v>1.7013990457497297E-2</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
-        <v>41487</v>
+        <v>41518</v>
       </c>
       <c r="B117" s="2">
-        <v>1.5599999999999999E-2</v>
+        <v>-4.4281628964232933E-2</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
-        <v>41518</v>
+        <v>41548</v>
       </c>
       <c r="B118" s="2">
-        <v>6.4600000000000005E-2</v>
+        <v>1.6995466262328174E-2</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
-        <v>41548</v>
+        <v>41579</v>
       </c>
       <c r="B119" s="2">
-        <v>3.8699999999999998E-2</v>
+        <v>5.0850894932710555E-2</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
-        <v>41579</v>
+        <v>41609</v>
       </c>
       <c r="B120" s="2">
-        <v>-9.4999999999999998E-3</v>
+        <v>-5.7941784535988528E-2</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
-        <v>41609</v>
+        <v>41640</v>
       </c>
       <c r="B121" s="2">
-        <v>4.19E-2</v>
+        <v>9.1674304116874827E-2</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
-        <v>41640</v>
+        <v>41671</v>
       </c>
       <c r="B122" s="2">
-        <v>-5.67E-2</v>
+        <v>-9.0869154335253444E-2</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
-        <v>41671</v>
+        <v>41699</v>
       </c>
       <c r="B123" s="2">
-        <v>5.7500000000000002E-2</v>
+        <v>1.7119064368083636E-2</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
-        <v>41699</v>
+        <v>41730</v>
       </c>
       <c r="B124" s="2">
-        <v>3.1899999999999998E-2</v>
+        <v>2.3581221906628702E-2</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
-        <v>41730</v>
+        <v>41760</v>
       </c>
       <c r="B125" s="2">
-        <v>9.9000000000000008E-3</v>
+        <v>7.5947319558662407E-3</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
-        <v>41760</v>
+        <v>41791</v>
       </c>
       <c r="B126" s="2">
-        <v>8.6999999999999994E-3</v>
+        <v>-1.9301876975067245E-2</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
-        <v>41791</v>
+        <v>41821</v>
       </c>
       <c r="B127" s="2">
-        <v>4.1300000000000003E-2</v>
+        <v>9.832912778544145E-3</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
-        <v>41821</v>
+        <v>41852</v>
       </c>
       <c r="B128" s="2">
-        <v>1.7399999999999999E-2</v>
+        <v>-1.659392676749416E-3</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
-        <v>41852</v>
+        <v>41883</v>
       </c>
       <c r="B129" s="2">
-        <v>1.5299999999999999E-2</v>
+        <v>2.0551910142236673E-2</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
-        <v>41883</v>
+        <v>41913</v>
       </c>
       <c r="B130" s="2">
-        <v>-1.4500000000000001E-2</v>
+        <v>-6.965073492611018E-2</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
-        <v>41913</v>
+        <v>41944</v>
       </c>
       <c r="B131" s="2">
-        <v>4.5400000000000003E-2</v>
+        <v>1.4250764424177831E-2</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
-        <v>41944</v>
+        <v>41974</v>
       </c>
       <c r="B132" s="2">
-        <v>1.4E-2</v>
+        <v>-2.3409193623802338E-4</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
-        <v>41974</v>
+        <v>42005</v>
       </c>
       <c r="B133" s="2">
-        <v>6.4000000000000003E-3</v>
+        <v>-6.1141420537201396E-2</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
-        <v>42005</v>
+        <v>42036</v>
       </c>
       <c r="B134" s="2">
-        <v>6.3899999999999998E-2</v>
+        <v>4.3228472940032514E-2</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
-        <v>42036</v>
+        <v>42064</v>
       </c>
       <c r="B135" s="2">
-        <v>-3.5999999999999999E-3</v>
+        <v>9.0792255378584485E-3</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
-        <v>42064</v>
+        <v>42095</v>
       </c>
       <c r="B136" s="2">
-        <v>1.66E-2</v>
+        <v>-2.5534646197234778E-2</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
-        <v>42095</v>
+        <v>42125</v>
       </c>
       <c r="B137" s="2">
-        <v>2.63E-2</v>
+        <v>0.10405598829392315</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
-        <v>42125</v>
+        <v>42156</v>
       </c>
       <c r="B138" s="2">
-        <v>-0.06</v>
+        <v>-5.6926448187005652E-2</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
-        <v>42156</v>
+        <v>42186</v>
       </c>
       <c r="B139" s="2">
-        <v>8.3000000000000001E-3</v>
+        <v>-1.4247507574320029E-2</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
-        <v>42186</v>
+        <v>42217</v>
       </c>
       <c r="B140" s="2">
-        <v>1.9400000000000001E-2</v>
+        <v>2.8440290924177214E-2</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
-        <v>42217</v>
+        <v>42248</v>
       </c>
       <c r="B141" s="2">
-        <v>-2.7799999999999998E-2</v>
+        <v>-3.0918236380800268E-2</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
-        <v>42248</v>
+        <v>42278</v>
       </c>
       <c r="B142" s="2">
-        <v>-2.0000000000000001E-4</v>
+        <v>-8.858968942720491E-2</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
-        <v>42278</v>
+        <v>42309</v>
       </c>
       <c r="B143" s="2">
-        <v>7.7899999999999997E-2</v>
+        <v>7.0766205884789102E-2</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
-        <v>42309</v>
+        <v>42339</v>
       </c>
       <c r="B144" s="2">
-        <v>-1.8E-3</v>
+        <v>-1.0626751813208934E-2</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
-        <v>42339</v>
+        <v>42370</v>
       </c>
       <c r="B145" s="2">
-        <v>-2.0199999999999999E-2</v>
+        <v>-3.9894464736215385E-3</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
-        <v>42370</v>
+        <v>42401</v>
       </c>
       <c r="B146" s="2">
-        <v>-2.52E-2</v>
+        <v>-2.0477911157332884E-2</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
-        <v>42401</v>
+        <v>42430</v>
       </c>
       <c r="B147" s="2">
-        <v>5.9999999999999995E-4</v>
+        <v>-5.7829213534752899E-2</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
-        <v>42430</v>
+        <v>42461</v>
       </c>
       <c r="B148" s="2">
-        <v>6.3299999999999995E-2</v>
+        <v>5.1745211409879088E-2</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
-        <v>42461</v>
+        <v>42491</v>
       </c>
       <c r="B149" s="2">
-        <v>0.03</v>
+        <v>3.7798123430747954E-2</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" s="1">
-        <v>42491</v>
+        <v>42522</v>
       </c>
       <c r="B150" s="2">
-        <v>-2.0899999999999998E-2</v>
+        <v>2.8431569224975695E-2</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" s="1">
-        <v>42522</v>
+        <v>42552</v>
       </c>
       <c r="B151" s="2">
-        <v>-2.5700000000000001E-2</v>
+        <v>-5.8401865889923021E-2</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" s="1">
-        <v>42552</v>
+        <v>42583</v>
       </c>
       <c r="B152" s="2">
-        <v>4.6699999999999998E-2</v>
+        <v>7.6879229150565997E-2</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" s="1">
-        <v>42583</v>
+        <v>42614</v>
       </c>
       <c r="B153" s="2">
-        <v>-5.4100000000000002E-2</v>
+        <v>-4.2417777656383882E-2</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" s="1">
-        <v>42614</v>
+        <v>42644</v>
       </c>
       <c r="B154" s="2">
-        <v>2.6599999999999999E-2</v>
+        <v>1.5285375168238691E-2</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" s="1">
-        <v>42644</v>
+        <v>42675</v>
       </c>
       <c r="B155" s="2">
-        <v>-2.3599999999999999E-2</v>
+        <v>-2.0524116424606165E-2</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" s="1">
-        <v>42675</v>
+        <v>42705</v>
       </c>
       <c r="B156" s="2">
-        <v>-5.4000000000000003E-3</v>
+        <v>-3.6266136175004182E-2</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" s="1">
-        <v>42705</v>
+        <v>42736</v>
       </c>
       <c r="B157" s="2">
-        <v>1.9800000000000002E-2</v>
+        <v>9.4729825638120158E-3</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
-        <v>42736</v>
+        <v>42767</v>
       </c>
       <c r="B158" s="2">
-        <v>1.41E-2</v>
+        <v>3.6377025012407471E-2</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
-        <v>42767</v>
+        <v>42795</v>
       </c>
       <c r="B159" s="2">
-        <v>-1.35E-2</v>
+        <v>-2.8323935086857266E-2</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
-        <v>42795</v>
+        <v>42826</v>
       </c>
       <c r="B160" s="2">
-        <v>1.37E-2</v>
+        <v>-1.3129493866857578E-2</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" s="1">
-        <v>42826</v>
+        <v>42856</v>
       </c>
       <c r="B161" s="2">
-        <v>2.86E-2</v>
+        <v>4.464801462824719E-2</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
-        <v>42856</v>
+        <v>42887</v>
       </c>
       <c r="B162" s="2">
-        <v>-9.4000000000000004E-3</v>
+        <v>2.7327472636344385E-2</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="1">
-        <v>42887</v>
+        <v>42917</v>
       </c>
       <c r="B163" s="2">
-        <v>-3.5099999999999999E-2</v>
+        <v>-9.0713810465117284E-2</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" s="1">
-        <v>42917</v>
+        <v>42948</v>
       </c>
       <c r="B164" s="2">
-        <v>5.4899999999999997E-2</v>
+        <v>2.6796139761780635E-2</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
-        <v>42948</v>
+        <v>42979</v>
       </c>
       <c r="B165" s="2">
-        <v>2.6200000000000001E-2</v>
+        <v>4.0437393316128389E-2</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" s="1">
-        <v>42979</v>
+        <v>43009</v>
       </c>
       <c r="B166" s="2">
-        <v>-1.44E-2</v>
+        <v>-7.9641751780014869E-2</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" s="1">
-        <v>43009</v>
+        <v>43040</v>
       </c>
       <c r="B167" s="2">
-        <v>6.0499999999999998E-2</v>
+        <v>2.1411416951962581E-2</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" s="1">
-        <v>43040</v>
+        <v>43070</v>
       </c>
       <c r="B168" s="2">
-        <v>2.7400000000000001E-2</v>
+        <v>1.7300694821265505E-2</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" s="1">
-        <v>43070</v>
+        <v>43101</v>
       </c>
       <c r="B169" s="2">
-        <v>7.3000000000000001E-3</v>
+        <v>2.1387211863309163E-2</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" s="1">
-        <v>43101</v>
+        <v>43132</v>
       </c>
       <c r="B170" s="2">
-        <v>-1.23E-2</v>
+        <v>-4.8041168055434902E-3</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" s="1">
-        <v>43132</v>
+        <v>43160</v>
       </c>
       <c r="B171" s="2">
-        <v>4.0000000000000002E-4</v>
+        <v>3.2698352092088379E-2</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" s="1">
-        <v>43160</v>
+        <v>43191</v>
       </c>
       <c r="B172" s="2">
-        <v>-4.0599999999999997E-2</v>
+        <v>-6.7913424303511882E-2</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" s="1">
-        <v>43191</v>
+        <v>43221</v>
       </c>
       <c r="B173" s="2">
-        <v>2.8899999999999999E-2</v>
+        <v>9.2467541925500107E-2</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" s="1">
-        <v>43221</v>
+        <v>43252</v>
       </c>
       <c r="B174" s="2">
-        <v>-5.1900000000000002E-2</v>
+        <v>-5.5560121713865485E-2</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" s="1">
-        <v>43252</v>
+        <v>43282</v>
       </c>
       <c r="B175" s="2">
-        <v>2.3999999999999998E-3</v>
+        <v>-6.3369701325601824E-3</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" s="1">
-        <v>43282</v>
+        <v>43313</v>
       </c>
       <c r="B176" s="2">
-        <v>1.29E-2</v>
+        <v>-1.9317994108669634E-3</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" s="1">
-        <v>43313</v>
+        <v>43344</v>
       </c>
       <c r="B177" s="2">
-        <v>1.6400000000000001E-2</v>
+        <v>4.0547943944886811E-2</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" s="1">
-        <v>43344</v>
+        <v>43374</v>
       </c>
       <c r="B178" s="2">
-        <v>-2.8299999999999999E-2</v>
+        <v>3.9139043964345754E-3</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" s="1">
-        <v>43374</v>
+        <v>43405</v>
       </c>
       <c r="B179" s="2">
-        <v>-4.6199999999999998E-2</v>
+        <v>9.2103182269396289E-3</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" s="1">
-        <v>43405</v>
+        <v>43435</v>
       </c>
       <c r="B180" s="2">
-        <v>-5.5300000000000002E-2</v>
+        <v>-5.0697064410723303E-2</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" s="1">
-        <v>43435</v>
+        <v>43466</v>
       </c>
       <c r="B181" s="2">
-        <v>3.3799999999999997E-2</v>
+        <v>-7.7302731907948896E-3</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" s="1">
-        <v>43466</v>
+        <v>43497</v>
       </c>
       <c r="B182" s="2">
-        <v>3.3599999999999998E-2</v>
+        <v>7.8170541384632308E-3</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" s="1">
-        <v>43497</v>
+        <v>43525</v>
       </c>
       <c r="B183" s="2">
-        <v>1.9900000000000001E-2</v>
+        <v>-3.8798676999387549E-3</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" s="1">
-        <v>43525</v>
+        <v>43556</v>
       </c>
       <c r="B184" s="2">
-        <v>1.6199999999999999E-2</v>
+        <v>-1.419221520291658E-2</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" s="1">
-        <v>43556</v>
+        <v>43586</v>
       </c>
       <c r="B185" s="2">
-        <v>1.24E-2</v>
+        <v>9.2025717521067252E-2</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" s="1">
-        <v>43586</v>
+        <v>43617</v>
       </c>
       <c r="B186" s="2">
-        <v>-4.2000000000000003E-2</v>
+        <v>-0.10650839330278583</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" s="1">
-        <v>43617</v>
+        <v>43647</v>
       </c>
       <c r="B187" s="2">
-        <v>5.8999999999999997E-2</v>
+        <v>5.8640633986491109E-2</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" s="1">
-        <v>43647</v>
+        <v>43678</v>
       </c>
       <c r="B188" s="2">
-        <v>-2.98E-2</v>
+        <v>-3.4856590883986627E-2</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" s="1">
-        <v>43678</v>
+        <v>43709</v>
       </c>
       <c r="B189" s="2">
-        <v>3.5999999999999999E-3</v>
+        <v>-2.0593179003691953E-2</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" s="1">
-        <v>43709</v>
+        <v>43739</v>
       </c>
       <c r="B190" s="2">
-        <v>-6.4000000000000003E-3</v>
+        <v>-6.1380098155280782E-2</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" s="1">
-        <v>43739</v>
+        <v>43770</v>
       </c>
       <c r="B191" s="2">
-        <v>6.8099999999999994E-2</v>
+        <v>5.2595759104122841E-2</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" s="1">
-        <v>43770</v>
+        <v>43800</v>
       </c>
       <c r="B192" s="2">
-        <v>-1.6199999999999999E-2</v>
+        <v>-6.689547183775113E-2</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" s="1">
-        <v>43800</v>
+        <v>43831</v>
       </c>
       <c r="B193" s="2">
-        <v>5.2200000000000003E-2</v>
+        <v>3.2601866496777987E-2</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" s="1">
-        <v>43831</v>
+        <v>43862</v>
       </c>
       <c r="B194" s="2">
-        <v>-1.6999999999999999E-3</v>
+        <v>6.3806912162248097E-2</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" s="1">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="B195" s="2">
-        <v>-8.9499999999999996E-2</v>
+        <v>-4.567084095725038E-3</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" s="1">
-        <v>43891</v>
+        <v>43922</v>
       </c>
       <c r="B196" s="2">
-        <v>-9.0899999999999995E-2</v>
+        <v>-0.29845386878833535</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" s="1">
-        <v>43922</v>
+        <v>43952</v>
       </c>
       <c r="B197" s="2">
-        <v>0.13159999999999999</v>
+        <v>0.12086592586010592</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" s="1">
-        <v>43952</v>
+        <v>43983</v>
       </c>
       <c r="B198" s="2">
-        <v>2.0899999999999998E-2</v>
+        <v>-7.8837000911847754E-2</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" s="1">
-        <v>43983</v>
+        <v>44013</v>
       </c>
       <c r="B199" s="2">
-        <v>7.4700000000000003E-2</v>
+        <v>-8.4874751502210799E-3</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" s="1">
-        <v>44013</v>
+        <v>44044</v>
       </c>
       <c r="B200" s="2">
-        <v>7.8299999999999995E-2</v>
+        <v>3.2973294141000253E-2</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" s="1">
-        <v>44044</v>
+        <v>44075</v>
       </c>
       <c r="B201" s="2">
-        <v>-2.8999999999999998E-3</v>
+        <v>3.3502596591721057E-2</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" s="1">
-        <v>44075</v>
+        <v>44105</v>
       </c>
       <c r="B202" s="2">
-        <v>-4.2299999999999997E-2</v>
+        <v>3.7635708894721787E-2</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" s="1">
-        <v>44105</v>
+        <v>44136</v>
       </c>
       <c r="B203" s="2">
-        <v>-4.8300000000000003E-2</v>
+        <v>-7.7736515078262181E-2</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" s="1">
-        <v>44136</v>
+        <v>44166</v>
       </c>
       <c r="B204" s="2">
-        <v>3.5299999999999998E-2</v>
+        <v>4.0508396403227342E-2</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" s="1">
-        <v>44166</v>
+        <v>44197</v>
       </c>
       <c r="B205" s="2">
-        <v>6.3299999999999995E-2</v>
+        <v>4.6300511458539306E-2</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" s="1">
-        <v>44197</v>
+        <v>44228</v>
       </c>
       <c r="B206" s="2">
-        <v>8.3999999999999995E-3</v>
+        <v>-4.5945383531687423E-2</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" s="1">
-        <v>44228</v>
+        <v>44256</v>
       </c>
       <c r="B207" s="2">
-        <v>7.6700000000000004E-2</v>
+        <v>-6.7721767698685209E-3</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" s="1">
-        <v>44256</v>
+        <v>44287</v>
       </c>
       <c r="B208" s="2">
-        <v>6.0100000000000001E-2</v>
+        <v>3.5342470210262045E-2</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" s="1">
-        <v>44287</v>
+        <v>44317</v>
       </c>
       <c r="B209" s="2">
-        <v>1.8E-3</v>
+        <v>-7.5933803434180547E-3</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" s="1">
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="B210" s="2">
-        <v>1.5699999999999999E-2</v>
+        <v>4.6455994578506687E-2</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" s="1">
-        <v>44348</v>
+        <v>44378</v>
       </c>
       <c r="B211" s="2">
-        <v>-1.72E-2</v>
+        <v>-6.1192992083298869E-2</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" s="1">
-        <v>44378</v>
+        <v>44409</v>
       </c>
       <c r="B212" s="2">
-        <v>3.1E-2</v>
+        <v>-1.2292954602975525E-2</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" s="1">
-        <v>44409</v>
+        <v>44440</v>
       </c>
       <c r="B213" s="2">
-        <v>3.8199999999999998E-2</v>
+        <v>1.9023256139773848E-2</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" s="1">
-        <v>44440</v>
+        <v>44470</v>
       </c>
       <c r="B214" s="2">
-        <v>1.1999999999999999E-3</v>
+        <v>1.2873719946114304E-2</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" s="1">
-        <v>44470</v>
+        <v>44501</v>
       </c>
       <c r="B215" s="2">
-        <v>-2.7E-2</v>
+        <v>2.4387959053673303E-2</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" s="1">
-        <v>44501</v>
+        <v>44531</v>
       </c>
       <c r="B216" s="2">
-        <v>2.5000000000000001E-3</v>
+        <v>-2.5891171784299338E-2</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" s="1">
-        <v>44531</v>
+        <v>44562</v>
       </c>
       <c r="B217" s="2">
-        <v>3.5299999999999998E-2</v>
+        <v>3.6112513870121266E-3</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" s="1">
-        <v>44562</v>
+        <v>44593</v>
       </c>
       <c r="B218" s="2">
-        <v>4.4900000000000002E-2</v>
+        <v>-2.0973672731049442E-2</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" s="1">
-        <v>44593</v>
+        <v>44621</v>
       </c>
       <c r="B219" s="2">
-        <v>4.4900000000000002E-2</v>
+        <v>4.3749292275641061E-3</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" s="1">
-        <v>44621</v>
+        <v>44652</v>
       </c>
       <c r="B220" s="2">
-        <v>2.2499999999999999E-2</v>
+        <v>5.8044354919907115E-2</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" s="1">
-        <v>44652</v>
+        <v>44682</v>
       </c>
       <c r="B221" s="2">
-        <v>-4.3099999999999999E-2</v>
+        <v>-3.9467958745954101E-2</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222" s="1">
-        <v>44682</v>
+        <v>44713</v>
       </c>
       <c r="B222" s="2">
-        <v>0</v>
+        <v>0.10903965539478289</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" s="1">
-        <v>44713</v>
+        <v>44743</v>
       </c>
       <c r="B223" s="2">
-        <v>-0.1036</v>
+        <v>-0.10589948075639677</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" s="1">
-        <v>44743</v>
+        <v>44774</v>
       </c>
       <c r="B224" s="2">
-        <v>3.1099999999999999E-2</v>
+        <v>4.064711805213439E-2</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" s="1">
-        <v>44774</v>
+        <v>44805</v>
       </c>
       <c r="B225" s="2">
-        <v>-1.23E-2</v>
+        <v>3.1200230652887462E-2</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" s="1">
-        <v>44805</v>
+        <v>44835</v>
       </c>
       <c r="B226" s="2">
-        <v>-4.4499999999999998E-2</v>
+        <v>-7.6781864395595201E-2</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" s="1">
-        <v>44835</v>
+        <v>44866</v>
       </c>
       <c r="B227" s="2">
-        <v>3.8399999999999997E-2</v>
+        <v>-1.3329778071933918E-2</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" s="1">
-        <v>44866</v>
+        <v>44896</v>
       </c>
       <c r="B228" s="2">
-        <v>6.6600000000000006E-2</v>
+        <v>0.1326344155621717</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" s="1">
-        <v>44896</v>
+        <v>44927</v>
       </c>
       <c r="B229" s="2">
-        <v>-3.6400000000000002E-2</v>
+        <v>-7.9555117679087961E-2</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" s="1">
-        <v>44927</v>
+        <v>44958</v>
       </c>
       <c r="B230" s="2">
-        <v>5.1499999999999997E-2</v>
+        <v>7.2721572413294466E-2</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" s="1">
-        <v>44958</v>
+        <v>44986</v>
       </c>
       <c r="B231" s="2">
-        <v>-3.0999999999999999E-3</v>
+        <v>2.3025630400421826E-2</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" s="1">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="B232" s="2">
-        <v>-4.6199999999999998E-2</v>
+        <v>-5.4617890941111247E-2</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" s="1">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="B233" s="2">
-        <v>3.5099999999999999E-2</v>
+        <v>7.2522721013071889E-2</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" s="1">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="B234" s="2">
-        <v>-3.8199999999999998E-2</v>
+        <v>-8.6923197372416938E-2</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="B235" s="2">
-        <v>2.8799999999999999E-2</v>
+        <v>7.7372006548137584E-4</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" s="1">
-        <v>45108</v>
+        <v>45139</v>
       </c>
       <c r="B236" s="2">
-        <v>3.7600000000000001E-2</v>
+        <v>6.2254486931552111E-2</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" s="1">
-        <v>45139</v>
+        <v>45170</v>
       </c>
       <c r="B237" s="2">
-        <v>-2.1000000000000001E-2</v>
+        <v>-2.3072693445519543E-2</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" s="1">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="B238" s="2">
-        <v>-2.4799999999999999E-2</v>
+        <v>2.9584589260012173E-3</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" s="1">
-        <v>45200</v>
+        <v>45231</v>
       </c>
       <c r="B239" s="2">
-        <v>-3.27E-2</v>
+        <v>-0.12918897582177347</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240" s="1">
-        <v>45231</v>
+        <v>45261</v>
       </c>
       <c r="B240" s="2">
-        <v>9.9900000000000003E-2</v>
+        <v>7.324632326658298E-2</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241" s="1">
-        <v>45261</v>
+        <v>45292</v>
       </c>
       <c r="B241" s="2">
-        <v>1.01E-2</v>
+        <v>4.5763103587928122E-2</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" s="1">
-        <v>45292</v>
+        <v>45323</v>
       </c>
       <c r="B242" s="2">
-        <v>-1.6799999999999999E-2</v>
+        <v>-1.0035664737985672E-2</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A243" s="1">
-        <v>45323</v>
-      </c>
-      <c r="B243" s="2">
-        <v>-1.84E-2</v>
+      <c r="B243">
+        <v>-2.2681286666709988E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2390,6 +2387,6 @@
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{70c52299-74de-4dfd-b117-c9c408edfa50}" enabled="1" method="Standard" siteId="{853cbaab-a620-4178-8933-88d76414184a}" removed="0"/>
+  <clbl:label id="{70c52299-74de-4dfd-b117-c9c408edfa50}" enabled="1" method="Standard" siteId="{853cbaab-a620-4178-8933-88d76414184a}" contentBits="0" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>